<commit_message>
TestNg Results added, UserDefinedFunctions class
</commit_message>
<xml_diff>
--- a/SC Store - automation framework/src/testData/testData.xlsx
+++ b/SC Store - automation framework/src/testData/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -397,18 +403,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="1" max="3" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -419,10 +427,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -432,7 +443,10 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>